<commit_message>
[JPADCADSandbox] More work on AircraftCADUtils.
</commit_message>
<xml_diff>
--- a/JPADSandBox_v2/out/AIRBUS A-320neo/BALANCE/Balance.xlsx
+++ b/JPADSandBox_v2/out/AIRBUS A-320neo/BALANCE/Balance.xlsx
@@ -15,13 +15,12 @@
     <sheet name="NACELLES" r:id="rId9" sheetId="7"/>
     <sheet name="POWER PLANT" r:id="rId10" sheetId="8"/>
     <sheet name="LANDING GEARS" r:id="rId11" sheetId="9"/>
-    <sheet name="SYSTEMS" r:id="rId12" sheetId="10"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="89">
   <si>
     <t>Description</t>
   </si>
@@ -257,12 +256,12 @@
     <t>Xcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
   </si>
   <si>
+    <t>TORENBEEK_1982</t>
+  </si>
+  <si>
     <t>SFORZA</t>
   </si>
   <si>
-    <t>TORENBEEK_1982</t>
-  </si>
-  <si>
     <t>Ycg LRF (semi-wing)</t>
   </si>
   <si>
@@ -288,33 +287,6 @@
   </si>
   <si>
     <t>Zcg ESTIMATION METHOD COMPARISON (WITHOUT CALIBRATIONS)</t>
-  </si>
-  <si>
-    <t>APU</t>
-  </si>
-  <si>
-    <t>Xcg BRF</t>
-  </si>
-  <si>
-    <t>Zcg BRF</t>
-  </si>
-  <si>
-    <t>AIR CONDITIONING AND ANTI-ICING SYSTEM</t>
-  </si>
-  <si>
-    <t>INSTRUMENTS AND NAVIGATION SYSTEM</t>
-  </si>
-  <si>
-    <t>HYDRAULIC AND PNEUMATIC SYSTEMS</t>
-  </si>
-  <si>
-    <t>ELECTRICAL SYSTEMS</t>
-  </si>
-  <si>
-    <t>CONTROL SURFACES</t>
-  </si>
-  <si>
-    <t>FURNISHINGS AND EQUIPMENTS</t>
   </si>
 </sst>
 </file>
@@ -410,7 +382,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="n">
-        <v>16.8190935117456</v>
+        <v>16.81194263315252</v>
       </c>
     </row>
     <row r="4">
@@ -432,7 +404,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.7693744630246111</v>
+        <v>-0.7698445289483744</v>
       </c>
     </row>
     <row r="6">
@@ -448,7 +420,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>37.01171160477802</v>
+        <v>36.84129117586568</v>
       </c>
     </row>
     <row r="8">
@@ -470,7 +442,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="n">
-        <v>-18.33580647134367</v>
+        <v>-18.347009127814765</v>
       </c>
     </row>
     <row r="10">
@@ -496,7 +468,7 @@
         <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>15.88011777493486</v>
+        <v>15.878438692483808</v>
       </c>
     </row>
     <row r="14">
@@ -518,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>-1.0920666475660572</v>
+        <v>-1.0911670762878014</v>
       </c>
     </row>
     <row r="16">
@@ -534,7 +506,7 @@
         <v>10</v>
       </c>
       <c r="C17" t="n">
-        <v>14.633951204770627</v>
+        <v>14.59393514971358</v>
       </c>
     </row>
     <row r="18">
@@ -556,7 +528,7 @@
         <v>10</v>
       </c>
       <c r="C19" t="n">
-        <v>-26.026237763157678</v>
+        <v>-26.004799093617713</v>
       </c>
     </row>
     <row r="20">
@@ -582,7 +554,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>15.309694761573756</v>
+        <v>15.878438692483808</v>
       </c>
     </row>
     <row r="24">
@@ -604,7 +576,7 @@
         <v>5</v>
       </c>
       <c r="C25" t="n">
-        <v>-0.8011335176628018</v>
+        <v>-1.0911670762878014</v>
       </c>
     </row>
     <row r="26">
@@ -620,7 +592,7 @@
         <v>10</v>
       </c>
       <c r="C27" t="n">
-        <v>1.0395748868042687</v>
+        <v>14.59393514971358</v>
       </c>
     </row>
     <row r="28">
@@ -642,7 +614,7 @@
         <v>10</v>
       </c>
       <c r="C29" t="n">
-        <v>-19.0926913272166</v>
+        <v>-26.004799093617713</v>
       </c>
     </row>
     <row r="30">
@@ -668,7 +640,7 @@
         <v>5</v>
       </c>
       <c r="C33" t="n">
-        <v>15.309694761573756</v>
+        <v>15.878438692483808</v>
       </c>
     </row>
     <row r="34">
@@ -690,7 +662,7 @@
         <v>5</v>
       </c>
       <c r="C35" t="n">
-        <v>-0.8011335176628018</v>
+        <v>-1.0911670762878014</v>
       </c>
     </row>
     <row r="36">
@@ -706,7 +678,7 @@
         <v>10</v>
       </c>
       <c r="C37" t="n">
-        <v>1.0395748868042687</v>
+        <v>14.59393514971358</v>
       </c>
     </row>
     <row r="38">
@@ -728,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="C39" t="n">
-        <v>-19.0926913272166</v>
+        <v>-26.004799093617713</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>15.842741007912934</v>
+        <v>16.241939578763954</v>
       </c>
     </row>
     <row r="44">
@@ -776,7 +748,7 @@
         <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>-0.580083303279513</v>
+        <v>-0.7729795977267571</v>
       </c>
     </row>
     <row r="46">
@@ -792,7 +764,7 @@
         <v>10</v>
       </c>
       <c r="C47" t="n">
-        <v>13.743184485084786</v>
+        <v>23.256923360672015</v>
       </c>
     </row>
     <row r="48">
@@ -814,7 +786,7 @@
         <v>10</v>
       </c>
       <c r="C49" t="n">
-        <v>-13.824601279820056</v>
+        <v>-18.421724389572724</v>
       </c>
     </row>
     <row r="50">
@@ -840,7 +812,7 @@
         <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>16.240721052005057</v>
+        <v>16.55473418354169</v>
       </c>
     </row>
     <row r="54">
@@ -862,7 +834,7 @@
         <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>-0.7505281159179367</v>
+        <v>-0.884907985523903</v>
       </c>
     </row>
     <row r="56">
@@ -878,7 +850,7 @@
         <v>10</v>
       </c>
       <c r="C57" t="n">
-        <v>23.227883313328192</v>
+        <v>30.711474576133213</v>
       </c>
     </row>
     <row r="58">
@@ -900,7 +872,7 @@
         <v>10</v>
       </c>
       <c r="C59" t="n">
-        <v>-17.886658507839332</v>
+        <v>-21.08921253212149</v>
       </c>
     </row>
     <row r="60">
@@ -921,7 +893,7 @@
         <v>10</v>
       </c>
       <c r="C62" t="n">
-        <v>-5.41823998557375</v>
+        <v>7.450424772207125</v>
       </c>
     </row>
     <row r="63">
@@ -932,7 +904,7 @@
         <v>10</v>
       </c>
       <c r="C63" t="n">
-        <v>23.227883313328192</v>
+        <v>30.711474576133213</v>
       </c>
     </row>
     <row r="64">
@@ -943,7 +915,7 @@
         <v>10</v>
       </c>
       <c r="C64" t="n">
-        <v>23.227883313328192</v>
+        <v>30.711474576133213</v>
       </c>
     </row>
     <row r="65">
@@ -974,7 +946,7 @@
         <v>53</v>
       </c>
       <c r="C69" t="n">
-        <v>82499.26556789856</v>
+        <v>72637.61007478533</v>
       </c>
     </row>
     <row r="70">
@@ -985,7 +957,7 @@
         <v>53</v>
       </c>
       <c r="C70" t="n">
-        <v>977096.3025434699</v>
+        <v>3109246.0899673</v>
       </c>
     </row>
     <row r="71">
@@ -996,7 +968,7 @@
         <v>53</v>
       </c>
       <c r="C71" t="n">
-        <v>1297717.9307699332</v>
+        <v>3036608.4798925156</v>
       </c>
     </row>
     <row r="72">
@@ -1039,336 +1011,7 @@
         <v>53</v>
       </c>
       <c r="C76" t="n">
-        <v>92090.81154390653</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="70"/>
-  <cols>
-    <col min="2" max="2" width="8.0" customWidth="true"/>
-    <col min="3" max="3" width="15.0" customWidth="true"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="n">
-        <v>27.397922499999993</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="n">
-        <v>13.634999999999998</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="n">
-        <v>-1.2399999999999998</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>90</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="n">
-        <v>3.0619549999999993</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" t="n">
-        <v>18.380866151069455</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="n">
-        <v>-0.8324576112167538</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
-        <v>90</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="n">
-        <v>9.879454999999997</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
-        <v>84</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
-        <v>91</v>
-      </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C25" t="n">
-        <v>-1.1374999999999995</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
-        <v>90</v>
-      </c>
-      <c r="B28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C28" t="n">
-        <v>15.134927463352513</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>84</v>
-      </c>
-      <c r="B29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>91</v>
-      </c>
-      <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" t="n">
-        <v>1.2762070139532358</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>90</v>
-      </c>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" t="n">
-        <v>15.065569999999994</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>84</v>
-      </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" t="n">
-        <v>1.0349999999999997</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>8</v>
+        <v>-31339.450165344497</v>
       </c>
     </row>
   </sheetData>
@@ -1608,7 +1251,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>15.763120357385809</v>
+        <v>16.342949999999995</v>
       </c>
     </row>
     <row r="24">
@@ -1619,7 +1262,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>16.342949999999995</v>
+        <v>15.763120357385809</v>
       </c>
     </row>
   </sheetData>
@@ -1859,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>4.192894429866952</v>
+        <v>3.581307767897423</v>
       </c>
     </row>
     <row r="24">
@@ -1870,7 +1513,7 @@
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>3.581307767897423</v>
+        <v>4.192894429866952</v>
       </c>
     </row>
     <row r="25">
@@ -1891,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="C27" t="n">
-        <v>5.130754833523566</v>
+        <v>6.24019727479847</v>
       </c>
     </row>
     <row r="28">
@@ -1902,7 +1545,7 @@
         <v>5</v>
       </c>
       <c r="C28" t="n">
-        <v>6.24019727479847</v>
+        <v>5.130754833523566</v>
       </c>
     </row>
   </sheetData>
@@ -2360,7 +2003,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2381,7 +2024,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -2621,7 +2264,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -2642,7 +2285,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
@@ -3122,7 +2765,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
@@ -3194,7 +2837,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>13.163099821788949</v>
+        <v>13.080400934931047</v>
       </c>
     </row>
     <row r="6">
@@ -3205,7 +2848,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>13.163099821788926</v>
+        <v>13.080400934931028</v>
       </c>
     </row>
     <row r="7">
@@ -3216,7 +2859,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="n">
-        <v>15.818400528151134</v>
+        <v>15.814930464711686</v>
       </c>
     </row>
     <row r="8">
@@ -3227,7 +2870,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="n">
-        <v>15.818400528151134</v>
+        <v>15.814930464711685</v>
       </c>
     </row>
     <row r="9">
@@ -3238,7 +2881,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="n">
-        <v>15.818400528151134</v>
+        <v>15.814930464711685</v>
       </c>
     </row>
     <row r="10">
@@ -3249,7 +2892,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="n">
-        <v>15.818400528151134</v>
+        <v>15.814930464711683</v>
       </c>
     </row>
     <row r="11">
@@ -3362,13 +3005,13 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>15.818400528151134</v>
+        <v>15.814930464711686</v>
       </c>
     </row>
     <row r="24">
@@ -3383,7 +3026,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>

</xml_diff>